<commit_message>
Changed interpolation to cubic hermite, added other interpolation tester.  Kyle
</commit_message>
<xml_diff>
--- a/LabVIEW/trunk/Instruments/Magna-Power Power Supply/Docs/Latest Magnet Calibration.xlsx
+++ b/LabVIEW/trunk/Instruments/Magna-Power Power Supply/Docs/Latest Magnet Calibration.xlsx
@@ -1933,13 +1933,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109994856"/>
-        <c:axId val="146918824"/>
+        <c:axId val="184477360"/>
+        <c:axId val="184477744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109994856"/>
+        <c:axId val="184477360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.1400000000000001"/>
+          <c:min val="0.43000000000000005"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1994,12 +1996,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146918824"/>
+        <c:crossAx val="184477744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146918824"/>
+        <c:axId val="184477744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,7 +2058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109994856"/>
+        <c:crossAx val="184477360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3942,11 +3944,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147246560"/>
-        <c:axId val="147256352"/>
+        <c:axId val="48041488"/>
+        <c:axId val="155659744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147246560"/>
+        <c:axId val="48041488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4003,12 +4005,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147256352"/>
+        <c:crossAx val="155659744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="147256352"/>
+        <c:axId val="155659744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4065,7 +4067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="147246560"/>
+        <c:crossAx val="48041488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5230,16 +5232,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5260,16 +5262,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5557,7 +5559,7 @@
   <dimension ref="A1:D289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C289" sqref="C2:C289"/>
+      <selection activeCell="A214" sqref="A214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>